<commit_message>
Remove AuditWbIn replaced with AuditWbOut
</commit_message>
<xml_diff>
--- a/src/test/resources/Integration Tests/Installed-Software.xlsx
+++ b/src/test/resources/Integration Tests/Installed-Software.xlsx
@@ -59,73 +59,73 @@
     <t>Test Vendor 1</t>
   </si>
   <si>
+    <t>Adobe</t>
+  </si>
+  <si>
+    <t>Cisco</t>
+  </si>
+  <si>
+    <t>Citrix</t>
+  </si>
+  <si>
+    <t>Fortinet</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Waves Audio</t>
+  </si>
+  <si>
+    <t>From Audit</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Accronym</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>ORC</t>
+  </si>
+  <si>
+    <t>WVS</t>
+  </si>
+  <si>
+    <t>TV1</t>
+  </si>
+  <si>
+    <t>CISC</t>
+  </si>
+  <si>
+    <t>CTRX</t>
+  </si>
+  <si>
+    <t>CNWS</t>
+  </si>
+  <si>
+    <t>FRT</t>
+  </si>
+  <si>
+    <t>CHKP</t>
+  </si>
+  <si>
+    <t>BOBJ</t>
+  </si>
+  <si>
+    <t>ADBE</t>
+  </si>
+  <si>
     <t>Test Vendor 2</t>
   </si>
   <si>
-    <t>Adobe</t>
-  </si>
-  <si>
-    <t>Cisco</t>
-  </si>
-  <si>
-    <t>Citrix</t>
-  </si>
-  <si>
-    <t>Fortinet</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>Waves Audio</t>
-  </si>
-  <si>
-    <t>From Audit</t>
-  </si>
-  <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Accronym</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>ORC</t>
-  </si>
-  <si>
-    <t>WVS</t>
-  </si>
-  <si>
-    <t>TV1</t>
-  </si>
-  <si>
     <t>TV2</t>
-  </si>
-  <si>
-    <t>CISC</t>
-  </si>
-  <si>
-    <t>CTRX</t>
-  </si>
-  <si>
-    <t>CNWS</t>
-  </si>
-  <si>
-    <t>FRT</t>
-  </si>
-  <si>
-    <t>CHKP</t>
-  </si>
-  <si>
-    <t>BOBJ</t>
-  </si>
-  <si>
-    <t>ADBE</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,13 +501,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -515,10 +515,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -529,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -540,7 +540,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -559,10 +559,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -570,10 +570,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -581,10 +581,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -595,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -603,10 +603,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -614,10 +614,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -625,10 +625,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -647,10 +647,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -661,18 +661,18 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>